<commit_message>
Updated all details of topics to be covered and daily progress
</commit_message>
<xml_diff>
--- a/NikhilBStudyPlan.xlsx
+++ b/NikhilBStudyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GCP Certification Plan" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="125">
   <si>
     <t>https://www.qwiklabs.com/</t>
   </si>
@@ -202,14 +202,210 @@
     <t>Hands on experience</t>
   </si>
   <si>
-    <t>1) Exploring GCP cloud Devops Engineering certification - Exam guide and coming up with an study plan for certification                                                                                                                                                                                                                          2) Created an Qwiklabs account - To enable hands on experience on fundamental features and capabalitied of GCP resources.                                                                                                                                                              Resoruce gathering for GCP -     for links to online resoruces, goto Learning resources sheets                                                                                                                                                                 3) Coverage -  Applying site reliability engineering principles to a service</t>
+    <t xml:space="preserve">1) SRE(Site relaible engineering) - Service layer objective(SLO), Service layer authentication(SLA), Service layer Indicator(SLI)                                                                                                                                                                                     2)Docker installation - on windows  iwth OS lower than windows 10 - use legacy docker tool box                                                                                                                                                                           2) Docker container - learning.oreilly.com     - Launching a docker container - starting based on Docker Image.                 </t>
+  </si>
+  <si>
+    <t>1) Exploring GCP cloud Devops Engineering certification  topics coverage - Exam guide and coming up with an study plan for certification                                                                                                                                                                                                                                                                                                                                                                                                                             2) Created an Qwiklabs account - To enable hands on experience on fundamental features and capabalitied of GCP resources.                                                                                                                                              Google cloud console - exploring key features, service menu items, API                                                                                                                                                         Resoruce gathering for GCP -     for links to online resoruces, goto Learning resources sheets                                                                                                                                                                 3) Coverage -  Applying site reliability engineering principles to a service</t>
+  </si>
+  <si>
+    <t>Site recovery</t>
+  </si>
+  <si>
+    <t>Devops</t>
+  </si>
+  <si>
+    <t>Apply Site reliability engineering principles to a service</t>
+  </si>
+  <si>
+    <t>Optimize service performance</t>
+  </si>
+  <si>
+    <t>Implement service monitoring strategies</t>
+  </si>
+  <si>
+    <t>Build and implement CI/CD pipeline for service</t>
+  </si>
+  <si>
+    <t>Manage service incidents</t>
+  </si>
+  <si>
+    <t>Stackdrivers, cloud build, kubernetes, kubernetes engine,Container registry</t>
+  </si>
+  <si>
+    <t>Operations and development perspective</t>
+  </si>
+  <si>
+    <t>End goal is to avoid any multi config, cluster management, build tools…</t>
+  </si>
+  <si>
+    <t>Top 10 things to know:</t>
+  </si>
+  <si>
+    <t>SRE - clear difference between SRO, SRA, SRI</t>
+  </si>
+  <si>
+    <t>Kubernetes Engine</t>
+  </si>
+  <si>
+    <t>Kubectle, gcloud cli commands</t>
+  </si>
+  <si>
+    <t>Error codes in 403/404 contexts</t>
+  </si>
+  <si>
+    <t>Complementary services around containers and kubes</t>
+  </si>
+  <si>
+    <t>Container complimentary services are</t>
+  </si>
+  <si>
+    <t>Google container registry</t>
+  </si>
+  <si>
+    <t>Easy to store and access private docker images in GCP. Easy to push and pull</t>
+  </si>
+  <si>
+    <t>Google cloud build</t>
+  </si>
+  <si>
+    <t>Deploy your containers on kubernetes cloud engine without needing t osetup authentication</t>
+  </si>
+  <si>
+    <t>Google Source Repositories</t>
+  </si>
+  <si>
+    <t>A single place to store, manage, and track code. Private Github</t>
+  </si>
+  <si>
+    <t>1) GCP Services - computation - App Engine Resource - spin a VM in GC console - create a enginex image inside the docker container - pull a source code into the Cloud SDK - deploy and retire the service                                           2) As part of Managing  a GC service - introduce a new service, deploy and retire it                                                     3) Create a Gcloud resource instance - Spin a VM using Gcloud console</t>
+  </si>
+  <si>
+    <t>Stack Drivers</t>
+  </si>
+  <si>
+    <t>StackDriver logging setup</t>
+  </si>
+  <si>
+    <t>setup alerts</t>
+  </si>
+  <si>
+    <t>Very Important</t>
+  </si>
+  <si>
+    <t>Difference between stakcdriver modules</t>
+  </si>
+  <si>
+    <t>Workflows - Debug and trace heavily tested</t>
+  </si>
+  <si>
+    <t>Difference between debug vs trace vs profiler</t>
+  </si>
+  <si>
+    <t>Stackdriver logging</t>
+  </si>
+  <si>
+    <t>Life of a log</t>
+  </si>
+  <si>
+    <t>Log entry</t>
+  </si>
+  <si>
+    <t>Logging API</t>
+  </si>
+  <si>
+    <t>Exprort</t>
+  </si>
+  <si>
+    <t>log into Stack driver logging</t>
+  </si>
+  <si>
+    <t>Billing is calculated based on logs ingested</t>
+  </si>
+  <si>
+    <t>Cloud logging commands to know</t>
+  </si>
+  <si>
+    <t>gcloud logging</t>
+  </si>
+  <si>
+    <t>gcloud logging log lists</t>
+  </si>
+  <si>
+    <t>gcloud logging sinks create</t>
+  </si>
+  <si>
+    <t>Export logs need to know</t>
+  </si>
+  <si>
+    <t>Cloud Storage</t>
+  </si>
+  <si>
+    <t>Cloud Pub/Sub</t>
+  </si>
+  <si>
+    <t>Big query</t>
+  </si>
+  <si>
+    <t>VPC Flow logs</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/vpc/docs/using-flow-logs</t>
+  </si>
+  <si>
+    <t>Handling Incidents</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/security/incident-response/</t>
+  </si>
+  <si>
+    <t>https://landing.google.com/sre/workbook/chapters/incident-response/</t>
+  </si>
+  <si>
+    <t>The main roles in incident response are the Incident Commander (IC), Communications Lead (CL), and Operations or Ops Lead (OL). IMAG organizes these roles into a hierarchy: the IC leads the incident response, and the CL and OL report to the IC.</t>
+  </si>
+  <si>
+    <t>Securing the pipelines. Container Security = Vulnerability analysis with Container Registry, Cloud Security Scanner</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/container-registry/docs/get-image-vulnerabilities</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/containers/security/</t>
+  </si>
+  <si>
+    <t>Kubernetes Engine uses what? Binary Authorization — you can require images to be signed by trusted authorities during the development process and then enforce signature validation when deploying.
+By enforcing validation, you can gain tighter control over your container environment by ensuring only verified images are integrated into the build-and-release process.</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/binary-authorization/</t>
+  </si>
+  <si>
+    <t>Load Balancing and Endpoints
+Know the basics of both VM and Container load balancing. What are instance groups.
+Know what Endpoints are and how the network policy is a specification of how groups of pods are allowed to communicate with each other and other network endpoints</t>
+  </si>
+  <si>
+    <t>https://kubernetes.io/docs/concepts/services-networking/</t>
+  </si>
+  <si>
+    <t>Infrastructure as Code (IaC)</t>
+  </si>
+  <si>
+    <t>Cloud Deployment Manager and Terraform were two areas that you may to understand.
+In Cloud Deployment Manager -Preview configuration
+gcloud deployment-manager deployments create example-deployment -config configuration-file.yaml \ -preview</t>
+  </si>
+  <si>
+    <t>Deploying a containerized application to Kubernetes Engine
+Cloud Build, Know your build steps, Automatic vs manual and integrate with Cloud Repositories. Custom builds steps (Memorize). Speed Up Builds and CI Pipelines
+Know how to deploy a containerized app and the details ..</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,8 +427,47 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF292929"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +486,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -265,7 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -274,6 +515,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -289,6 +543,176 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Image for post"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="19211925"/>
+          <a:ext cx="6096000" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Image for post"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="23879175"/>
+          <a:ext cx="6096000" cy="2905125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Image for post"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="28498800"/>
+          <a:ext cx="6096000" cy="4905375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -581,7 +1005,7 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +1253,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,31 +1340,342 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="81.28515625" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A51" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="112.5" x14ac:dyDescent="0.3">
+      <c r="A73" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A92" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="A93" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="A111" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A52" r:id="rId1"/>
+    <hyperlink ref="A56" r:id="rId2"/>
+    <hyperlink ref="A57" r:id="rId3"/>
+    <hyperlink ref="A62" r:id="rId4"/>
+    <hyperlink ref="A64" r:id="rId5"/>
+    <hyperlink ref="A66" r:id="rId6"/>
+    <hyperlink ref="A70" r:id="rId7"/>
+    <hyperlink ref="B73" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -948,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,17 +1698,23 @@
         <v>44025</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>44026</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>44027</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>